<commit_message>
finished transferring data from 2019 spring file.
</commit_message>
<xml_diff>
--- a/excel/CMC_Spring_2019_bookstore_list.xlsx
+++ b/excel/CMC_Spring_2019_bookstore_list.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="28125"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15520"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15460"/>
   </bookViews>
   <sheets>
     <sheet name="994 Spring 19 Booklist 01.24.19" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'994 Spring 19 Booklist 01.24.19'!$A$1:$M$661</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'994 Spring 19 Booklist 01.24.19'!$A$1:$M$660</definedName>
   </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3639" uniqueCount="1109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4150" uniqueCount="1112">
   <si>
     <t>Division</t>
   </si>
@@ -3355,6 +3355,15 @@
   </si>
   <si>
     <t>Used Rental Fee</t>
+  </si>
+  <si>
+    <t>Unique Dept</t>
+  </si>
+  <si>
+    <t>Unique Profs</t>
+  </si>
+  <si>
+    <t>Unique professor + course code = course</t>
   </si>
 </sst>
 </file>
@@ -3364,7 +3373,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3512,6 +3521,13 @@
       <u/>
       <sz val="11"/>
       <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -3814,7 +3830,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="44">
+  <cellStyleXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3859,8 +3875,32 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -3873,8 +3913,12 @@
     <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="44">
+  <cellStyles count="68">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="2" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="3" builtinId="38" customBuiltin="1"/>
@@ -3904,12 +3948,36 @@
     <cellStyle name="Check Cell" xfId="27" builtinId="23" customBuiltin="1"/>
     <cellStyle name="Explanatory Text" xfId="28" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Followed Hyperlink" xfId="43" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="45" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="47" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="49" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="51" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="53" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="55" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="57" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="59" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="61" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="63" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="65" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="67" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="29" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Heading 1" xfId="30" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 2" xfId="31" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="32" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="33" builtinId="19" customBuiltin="1"/>
     <cellStyle name="Hyperlink" xfId="42" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="44" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="46" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="48" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="50" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="52" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="54" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="56" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="58" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="60" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="62" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="64" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="66" builtinId="8" hidden="1"/>
     <cellStyle name="Input" xfId="34" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="35" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="36" builtinId="28" customBuiltin="1"/>
@@ -4254,13 +4322,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M663"/>
+  <dimension ref="A1:U663"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="O17" sqref="O17"/>
+      <selection pane="bottomRight" activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -4270,9 +4338,10 @@
     <col min="7" max="7" width="14.5" customWidth="1"/>
     <col min="8" max="8" width="36.83203125" customWidth="1"/>
     <col min="10" max="13" width="8.83203125" style="2"/>
+    <col min="19" max="19" width="13.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="3" customFormat="1" ht="48.75" customHeight="1">
+    <row r="1" spans="1:21" s="3" customFormat="1" ht="48.75" customHeight="1">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -4312,8 +4381,17 @@
       <c r="M1" s="5" t="s">
         <v>1108</v>
       </c>
-    </row>
-    <row r="2" spans="1:13">
+      <c r="O1" s="6" t="s">
+        <v>1109</v>
+      </c>
+      <c r="Q1" s="6" t="s">
+        <v>1110</v>
+      </c>
+      <c r="S1" s="6" t="s">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -4350,8 +4428,23 @@
       <c r="M2" s="2">
         <v>9.98</v>
       </c>
-    </row>
-    <row r="3" spans="1:13">
+      <c r="O2" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q2" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="S2" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="T2" s="7">
+        <v>125</v>
+      </c>
+      <c r="U2" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -4382,8 +4475,23 @@
       <c r="K3" s="2">
         <v>3.75</v>
       </c>
-    </row>
-    <row r="4" spans="1:13">
+      <c r="O3" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q3" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="S3" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="T3" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="U3" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -4420,8 +4528,23 @@
       <c r="M4" s="2">
         <v>7.68</v>
       </c>
-    </row>
-    <row r="5" spans="1:13">
+      <c r="O4" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q4" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="S4" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="T4" s="7">
+        <v>2</v>
+      </c>
+      <c r="U4" s="7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -4458,8 +4581,23 @@
       <c r="M5" s="2">
         <v>7.2</v>
       </c>
-    </row>
-    <row r="6" spans="1:13">
+      <c r="O5" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="Q5" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="S5" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="T5" s="7">
+        <v>44</v>
+      </c>
+      <c r="U5" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -4496,8 +4634,23 @@
       <c r="M6" s="2">
         <v>18.22</v>
       </c>
-    </row>
-    <row r="7" spans="1:13">
+      <c r="O6" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q6" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="S6" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="T6" s="7">
+        <v>140</v>
+      </c>
+      <c r="U6" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -4534,8 +4687,23 @@
       <c r="M7" s="2">
         <v>4.78</v>
       </c>
-    </row>
-    <row r="8" spans="1:13">
+      <c r="O7" s="7" t="s">
+        <v>242</v>
+      </c>
+      <c r="Q7" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="S7" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="T7" s="7">
+        <v>55</v>
+      </c>
+      <c r="U7" s="7" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -4566,8 +4734,23 @@
       <c r="K8" s="2">
         <v>21.75</v>
       </c>
-    </row>
-    <row r="9" spans="1:13">
+      <c r="O8" s="7" t="s">
+        <v>318</v>
+      </c>
+      <c r="Q8" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="S8" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="T8" s="7">
+        <v>50</v>
+      </c>
+      <c r="U8" s="7" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -4598,8 +4781,23 @@
       <c r="K9" s="2">
         <v>22.5</v>
       </c>
-    </row>
-    <row r="10" spans="1:13">
+      <c r="O9" s="7" t="s">
+        <v>319</v>
+      </c>
+      <c r="Q9" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="S9" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="T9" s="7">
+        <v>50</v>
+      </c>
+      <c r="U9" s="7" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -4636,8 +4834,23 @@
       <c r="M10" s="2">
         <v>40.799999999999997</v>
       </c>
-    </row>
-    <row r="11" spans="1:13">
+      <c r="O10" s="7" t="s">
+        <v>338</v>
+      </c>
+      <c r="Q10" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="S10" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="T10" s="7">
+        <v>65</v>
+      </c>
+      <c r="U10" s="7" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -4674,8 +4887,23 @@
       <c r="M11" s="2">
         <v>40.799999999999997</v>
       </c>
-    </row>
-    <row r="12" spans="1:13">
+      <c r="O11" s="7" t="s">
+        <v>402</v>
+      </c>
+      <c r="Q11" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="S11" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="T11" s="7">
+        <v>86</v>
+      </c>
+      <c r="U11" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -4712,8 +4940,23 @@
       <c r="M12" s="2">
         <v>40.799999999999997</v>
       </c>
-    </row>
-    <row r="13" spans="1:13">
+      <c r="O12" s="7" t="s">
+        <v>635</v>
+      </c>
+      <c r="Q12" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="S12" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="T12" s="7">
+        <v>86</v>
+      </c>
+      <c r="U12" s="7" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -4750,8 +4993,23 @@
       <c r="M13" s="2">
         <v>14.38</v>
       </c>
-    </row>
-    <row r="14" spans="1:13">
+      <c r="O13" s="7" t="s">
+        <v>779</v>
+      </c>
+      <c r="Q13" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="S13" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="T13" s="7">
+        <v>86</v>
+      </c>
+      <c r="U13" s="7" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -4791,8 +5049,23 @@
       <c r="M14" s="2">
         <v>40.799999999999997</v>
       </c>
-    </row>
-    <row r="15" spans="1:13">
+      <c r="O14" s="7" t="s">
+        <v>786</v>
+      </c>
+      <c r="Q14" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="S14" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="T14" s="7">
+        <v>98</v>
+      </c>
+      <c r="U14" s="7" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -4832,8 +5105,23 @@
       <c r="M15" s="2">
         <v>18.72</v>
       </c>
-    </row>
-    <row r="16" spans="1:13">
+      <c r="O15" s="7" t="s">
+        <v>789</v>
+      </c>
+      <c r="Q15" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="S15" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="T15" s="7">
+        <v>100</v>
+      </c>
+      <c r="U15" s="7" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21">
       <c r="A16" t="s">
         <v>12</v>
       </c>
@@ -4873,8 +5161,23 @@
       <c r="M16" s="2">
         <v>164.28</v>
       </c>
-    </row>
-    <row r="17" spans="1:13">
+      <c r="O16" s="7" t="s">
+        <v>881</v>
+      </c>
+      <c r="Q16" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="S16" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="T16" s="7">
+        <v>101</v>
+      </c>
+      <c r="U16" s="7" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21">
       <c r="A17" t="s">
         <v>12</v>
       </c>
@@ -4914,8 +5217,23 @@
       <c r="M17" s="2">
         <v>126.36</v>
       </c>
-    </row>
-    <row r="18" spans="1:13">
+      <c r="O17" s="7" t="s">
+        <v>908</v>
+      </c>
+      <c r="Q17" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="S17" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="T17" s="7">
+        <v>101</v>
+      </c>
+      <c r="U17" s="7" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21">
       <c r="A18" t="s">
         <v>12</v>
       </c>
@@ -4955,8 +5273,23 @@
       <c r="M18" s="2">
         <v>80.88</v>
       </c>
-    </row>
-    <row r="19" spans="1:13">
+      <c r="O18" s="7" t="s">
+        <v>941</v>
+      </c>
+      <c r="Q18" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="S18" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="T18" s="7">
+        <v>101</v>
+      </c>
+      <c r="U18" s="7" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21">
       <c r="A19" t="s">
         <v>12</v>
       </c>
@@ -4990,8 +5323,23 @@
       <c r="K19" s="2">
         <v>166.75</v>
       </c>
-    </row>
-    <row r="20" spans="1:13">
+      <c r="O19" s="7" t="s">
+        <v>945</v>
+      </c>
+      <c r="Q19" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="S19" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="T19" s="7">
+        <v>102</v>
+      </c>
+      <c r="U19" s="7" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21">
       <c r="A20" t="s">
         <v>12</v>
       </c>
@@ -5025,8 +5373,23 @@
       <c r="K20" s="2">
         <v>166.75</v>
       </c>
-    </row>
-    <row r="21" spans="1:13">
+      <c r="O20" s="7" t="s">
+        <v>998</v>
+      </c>
+      <c r="Q20" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="S20" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="T20" s="7">
+        <v>102</v>
+      </c>
+      <c r="U20" s="7" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21">
       <c r="A21" t="s">
         <v>12</v>
       </c>
@@ -5060,8 +5423,23 @@
       <c r="K21" s="2">
         <v>166.75</v>
       </c>
-    </row>
-    <row r="22" spans="1:13">
+      <c r="O21" s="7" t="s">
+        <v>1045</v>
+      </c>
+      <c r="Q21" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="S21" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="T21" s="7">
+        <v>120</v>
+      </c>
+      <c r="U21" s="7" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21">
       <c r="A22" t="s">
         <v>12</v>
       </c>
@@ -5095,8 +5473,23 @@
       <c r="K22" s="2">
         <v>166.75</v>
       </c>
-    </row>
-    <row r="23" spans="1:13">
+      <c r="O22" s="7" t="s">
+        <v>1084</v>
+      </c>
+      <c r="Q22" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="S22" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="T22" s="7">
+        <v>120</v>
+      </c>
+      <c r="U22" s="7" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21">
       <c r="A23" t="s">
         <v>12</v>
       </c>
@@ -5130,8 +5523,20 @@
       <c r="K23" s="2">
         <v>166.75</v>
       </c>
-    </row>
-    <row r="24" spans="1:13">
+      <c r="Q23" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="S23" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="T23" s="7">
+        <v>125</v>
+      </c>
+      <c r="U23" s="7" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21">
       <c r="A24" t="s">
         <v>12</v>
       </c>
@@ -5171,8 +5576,20 @@
       <c r="M24" s="2">
         <v>80.88</v>
       </c>
-    </row>
-    <row r="25" spans="1:13">
+      <c r="Q24" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="S24" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="T24" s="7">
+        <v>135</v>
+      </c>
+      <c r="U24" s="7" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21">
       <c r="A25" t="s">
         <v>12</v>
       </c>
@@ -5212,8 +5629,20 @@
       <c r="M25" s="2">
         <v>19.68</v>
       </c>
-    </row>
-    <row r="26" spans="1:13">
+      <c r="Q25" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="S25" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="T25" s="7">
+        <v>136</v>
+      </c>
+      <c r="U25" s="7" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21">
       <c r="A26" t="s">
         <v>12</v>
       </c>
@@ -5253,8 +5682,20 @@
       <c r="M26" s="2">
         <v>127.44</v>
       </c>
-    </row>
-    <row r="27" spans="1:13">
+      <c r="Q26" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="S26" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="T26" s="7">
+        <v>139</v>
+      </c>
+      <c r="U26" s="7" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21">
       <c r="A27" t="s">
         <v>12</v>
       </c>
@@ -5294,8 +5735,20 @@
       <c r="M27" s="2">
         <v>127.44</v>
       </c>
-    </row>
-    <row r="28" spans="1:13">
+      <c r="Q27" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="S27" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="T27" s="7">
+        <v>149</v>
+      </c>
+      <c r="U27" s="7" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21">
       <c r="A28" t="s">
         <v>12</v>
       </c>
@@ -5329,8 +5782,20 @@
       <c r="K28" s="2">
         <v>300.75</v>
       </c>
-    </row>
-    <row r="29" spans="1:13">
+      <c r="Q28" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="S28" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="T28" s="7">
+        <v>150</v>
+      </c>
+      <c r="U28" s="7" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21">
       <c r="A29" t="s">
         <v>12</v>
       </c>
@@ -5370,8 +5835,20 @@
       <c r="M29" s="2">
         <v>164.28</v>
       </c>
-    </row>
-    <row r="30" spans="1:13">
+      <c r="Q29" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="S29" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="T29" s="7">
+        <v>154</v>
+      </c>
+      <c r="U29" s="7" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21">
       <c r="A30" t="s">
         <v>12</v>
       </c>
@@ -5411,8 +5888,20 @@
       <c r="M30" s="2">
         <v>81.96</v>
       </c>
-    </row>
-    <row r="31" spans="1:13">
+      <c r="Q30" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="S30" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="T30" s="7">
+        <v>155</v>
+      </c>
+      <c r="U30" s="7" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21">
       <c r="A31" t="s">
         <v>12</v>
       </c>
@@ -5452,8 +5941,20 @@
       <c r="M31" s="2">
         <v>81.96</v>
       </c>
-    </row>
-    <row r="32" spans="1:13">
+      <c r="Q31" s="7" t="s">
+        <v>204</v>
+      </c>
+      <c r="S31" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="T31" s="7">
+        <v>156</v>
+      </c>
+      <c r="U31" s="7" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21">
       <c r="A32" t="s">
         <v>12</v>
       </c>
@@ -5493,8 +5994,20 @@
       <c r="M32" s="2">
         <v>127.44</v>
       </c>
-    </row>
-    <row r="33" spans="1:13">
+      <c r="Q32" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="S32" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="T32" s="7">
+        <v>160</v>
+      </c>
+      <c r="U32" s="7" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21">
       <c r="A33" t="s">
         <v>12</v>
       </c>
@@ -5528,8 +6041,20 @@
       <c r="K33" s="2">
         <v>300.75</v>
       </c>
-    </row>
-    <row r="34" spans="1:13">
+      <c r="Q33" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="S33" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="T33" s="7">
+        <v>165</v>
+      </c>
+      <c r="U33" s="7" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21">
       <c r="A34" t="s">
         <v>12</v>
       </c>
@@ -5569,8 +6094,20 @@
       <c r="M34" s="2">
         <v>164.28</v>
       </c>
-    </row>
-    <row r="35" spans="1:13">
+      <c r="Q34" s="7" t="s">
+        <v>251</v>
+      </c>
+      <c r="S34" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="T34" s="7">
+        <v>173</v>
+      </c>
+      <c r="U34" s="7" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21">
       <c r="A35" t="s">
         <v>12</v>
       </c>
@@ -5610,8 +6147,20 @@
       <c r="M35" s="2">
         <v>158.4</v>
       </c>
-    </row>
-    <row r="36" spans="1:13">
+      <c r="Q35" s="7" t="s">
+        <v>264</v>
+      </c>
+      <c r="S35" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="T35" s="7">
+        <v>175</v>
+      </c>
+      <c r="U35" s="7" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="36" spans="1:21">
       <c r="A36" t="s">
         <v>12</v>
       </c>
@@ -5651,8 +6200,20 @@
       <c r="M36" s="2">
         <v>158.4</v>
       </c>
-    </row>
-    <row r="37" spans="1:13">
+      <c r="Q36" s="7" t="s">
+        <v>279</v>
+      </c>
+      <c r="S36" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="T36" s="7">
+        <v>180</v>
+      </c>
+      <c r="U36" s="7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="37" spans="1:21">
       <c r="A37" t="s">
         <v>12</v>
       </c>
@@ -5692,8 +6253,20 @@
       <c r="M37" s="2">
         <v>158.4</v>
       </c>
-    </row>
-    <row r="38" spans="1:13">
+      <c r="Q37" s="7" t="s">
+        <v>285</v>
+      </c>
+      <c r="S37" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="T37" s="7">
+        <v>186</v>
+      </c>
+      <c r="U37" s="7" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="38" spans="1:21">
       <c r="A38" t="s">
         <v>12</v>
       </c>
@@ -5733,8 +6306,20 @@
       <c r="M38" s="2">
         <v>158.4</v>
       </c>
-    </row>
-    <row r="39" spans="1:13">
+      <c r="Q38" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="S38" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="T38" s="7">
+        <v>191</v>
+      </c>
+      <c r="U38" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="39" spans="1:21">
       <c r="A39" t="s">
         <v>12</v>
       </c>
@@ -5774,8 +6359,20 @@
       <c r="M39" s="2">
         <v>126.36</v>
       </c>
-    </row>
-    <row r="40" spans="1:13">
+      <c r="Q39" s="7" t="s">
+        <v>308</v>
+      </c>
+      <c r="S39" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="T39" s="7">
+        <v>198</v>
+      </c>
+      <c r="U39" s="7" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="40" spans="1:21">
       <c r="A40" t="s">
         <v>12</v>
       </c>
@@ -5815,8 +6412,20 @@
       <c r="M40" s="2">
         <v>126.36</v>
       </c>
-    </row>
-    <row r="41" spans="1:13">
+      <c r="Q40" s="7" t="s">
+        <v>320</v>
+      </c>
+      <c r="S40" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="T40" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="U40" s="7" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="41" spans="1:21">
       <c r="A41" t="s">
         <v>12</v>
       </c>
@@ -5856,8 +6465,20 @@
       <c r="M41" s="2">
         <v>126.36</v>
       </c>
-    </row>
-    <row r="42" spans="1:13">
+      <c r="Q41" s="7" t="s">
+        <v>325</v>
+      </c>
+      <c r="S41" s="7" t="s">
+        <v>242</v>
+      </c>
+      <c r="T41" s="7">
+        <v>10</v>
+      </c>
+      <c r="U41" s="7" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="42" spans="1:21">
       <c r="A42" t="s">
         <v>12</v>
       </c>
@@ -5897,8 +6518,20 @@
       <c r="M42" s="2">
         <v>126.36</v>
       </c>
-    </row>
-    <row r="43" spans="1:13">
+      <c r="Q42" s="7" t="s">
+        <v>339</v>
+      </c>
+      <c r="S42" s="7" t="s">
+        <v>242</v>
+      </c>
+      <c r="T42" s="7">
+        <v>10</v>
+      </c>
+      <c r="U42" s="7" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="43" spans="1:21">
       <c r="A43" t="s">
         <v>12</v>
       </c>
@@ -5932,8 +6565,20 @@
       <c r="K43" s="2">
         <v>153</v>
       </c>
-    </row>
-    <row r="44" spans="1:13">
+      <c r="Q43" s="7" t="s">
+        <v>357</v>
+      </c>
+      <c r="S43" s="7" t="s">
+        <v>242</v>
+      </c>
+      <c r="T43" s="7">
+        <v>10</v>
+      </c>
+      <c r="U43" s="7" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="44" spans="1:21">
       <c r="A44" t="s">
         <v>12</v>
       </c>
@@ -5967,8 +6612,20 @@
       <c r="K44" s="2">
         <v>153</v>
       </c>
-    </row>
-    <row r="45" spans="1:13">
+      <c r="Q44" s="7" t="s">
+        <v>240</v>
+      </c>
+      <c r="S44" s="7" t="s">
+        <v>242</v>
+      </c>
+      <c r="T44" s="7">
+        <v>10</v>
+      </c>
+      <c r="U44" s="7" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="45" spans="1:21">
       <c r="A45" t="s">
         <v>12</v>
       </c>
@@ -6002,8 +6659,20 @@
       <c r="K45" s="2">
         <v>125.25</v>
       </c>
-    </row>
-    <row r="46" spans="1:13">
+      <c r="Q45" s="7" t="s">
+        <v>369</v>
+      </c>
+      <c r="S45" s="7" t="s">
+        <v>242</v>
+      </c>
+      <c r="T45" s="7">
+        <v>10</v>
+      </c>
+      <c r="U45" s="7" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="46" spans="1:21">
       <c r="A46" t="s">
         <v>12</v>
       </c>
@@ -6037,8 +6706,20 @@
       <c r="K46" s="2">
         <v>252</v>
       </c>
-    </row>
-    <row r="47" spans="1:13">
+      <c r="Q46" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="S46" s="7" t="s">
+        <v>242</v>
+      </c>
+      <c r="T46" s="7">
+        <v>10</v>
+      </c>
+      <c r="U46" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="47" spans="1:21">
       <c r="A47" t="s">
         <v>12</v>
       </c>
@@ -6078,8 +6759,20 @@
       <c r="M47" s="2">
         <v>153.47999999999999</v>
       </c>
-    </row>
-    <row r="48" spans="1:13">
+      <c r="Q47" s="7" t="s">
+        <v>385</v>
+      </c>
+      <c r="S47" s="7" t="s">
+        <v>242</v>
+      </c>
+      <c r="T47" s="7">
+        <v>10</v>
+      </c>
+      <c r="U47" s="7" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="48" spans="1:21">
       <c r="A48" t="s">
         <v>12</v>
       </c>
@@ -6113,8 +6806,20 @@
       <c r="K48" s="2">
         <v>252</v>
       </c>
-    </row>
-    <row r="49" spans="1:13">
+      <c r="Q48" s="7" t="s">
+        <v>397</v>
+      </c>
+      <c r="S48" s="7" t="s">
+        <v>318</v>
+      </c>
+      <c r="T48" s="7">
+        <v>330</v>
+      </c>
+      <c r="U48" s="7" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="49" spans="1:21">
       <c r="A49" t="s">
         <v>12</v>
       </c>
@@ -6154,8 +6859,20 @@
       <c r="M49" s="2">
         <v>153.47999999999999</v>
       </c>
-    </row>
-    <row r="50" spans="1:13">
+      <c r="Q49" s="7" t="s">
+        <v>405</v>
+      </c>
+      <c r="S49" s="7" t="s">
+        <v>318</v>
+      </c>
+      <c r="T49" s="7">
+        <v>420</v>
+      </c>
+      <c r="U49" s="7" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="50" spans="1:21">
       <c r="A50" t="s">
         <v>12</v>
       </c>
@@ -6189,8 +6906,20 @@
       <c r="K50" s="2">
         <v>125.25</v>
       </c>
-    </row>
-    <row r="51" spans="1:13">
+      <c r="Q50" s="7" t="s">
+        <v>420</v>
+      </c>
+      <c r="S50" s="7" t="s">
+        <v>319</v>
+      </c>
+      <c r="T50" s="7">
+        <v>1</v>
+      </c>
+      <c r="U50" s="7" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="51" spans="1:21">
       <c r="A51" t="s">
         <v>12</v>
       </c>
@@ -6230,8 +6959,20 @@
       <c r="M51" s="2">
         <v>168.72</v>
       </c>
-    </row>
-    <row r="52" spans="1:13">
+      <c r="Q51" s="7" t="s">
+        <v>432</v>
+      </c>
+      <c r="S51" s="7" t="s">
+        <v>319</v>
+      </c>
+      <c r="T51" s="7">
+        <v>2</v>
+      </c>
+      <c r="U51" s="7" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="52" spans="1:21">
       <c r="A52" t="s">
         <v>12</v>
       </c>
@@ -6271,8 +7012,20 @@
       <c r="M52" s="2">
         <v>178.2</v>
       </c>
-    </row>
-    <row r="53" spans="1:13">
+      <c r="Q52" s="7" t="s">
+        <v>439</v>
+      </c>
+      <c r="S52" s="7" t="s">
+        <v>319</v>
+      </c>
+      <c r="T52" s="7">
+        <v>117</v>
+      </c>
+      <c r="U52" s="7" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="53" spans="1:21">
       <c r="A53" t="s">
         <v>12</v>
       </c>
@@ -6312,8 +7065,20 @@
       <c r="M53" s="2">
         <v>111.12</v>
       </c>
-    </row>
-    <row r="54" spans="1:13">
+      <c r="Q53" s="7" t="s">
+        <v>403</v>
+      </c>
+      <c r="S53" s="7" t="s">
+        <v>338</v>
+      </c>
+      <c r="T53" s="7">
+        <v>10</v>
+      </c>
+      <c r="U53" s="7" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="54" spans="1:21">
       <c r="A54" t="s">
         <v>12</v>
       </c>
@@ -6353,8 +7118,20 @@
       <c r="M54" s="2">
         <v>164.28</v>
       </c>
-    </row>
-    <row r="55" spans="1:13">
+      <c r="Q54" s="7" t="s">
+        <v>448</v>
+      </c>
+      <c r="S54" s="7" t="s">
+        <v>338</v>
+      </c>
+      <c r="T54" s="7">
+        <v>10</v>
+      </c>
+      <c r="U54" s="7" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="55" spans="1:21">
       <c r="A55" t="s">
         <v>12</v>
       </c>
@@ -6394,8 +7171,20 @@
       <c r="M55" s="2">
         <v>162.36000000000001</v>
       </c>
-    </row>
-    <row r="56" spans="1:13">
+      <c r="Q55" s="7" t="s">
+        <v>459</v>
+      </c>
+      <c r="S55" s="7" t="s">
+        <v>338</v>
+      </c>
+      <c r="T55" s="7">
+        <v>10</v>
+      </c>
+      <c r="U55" s="7" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="56" spans="1:21">
       <c r="A56" t="s">
         <v>12</v>
       </c>
@@ -6435,8 +7224,20 @@
       <c r="M56" s="2">
         <v>164.28</v>
       </c>
-    </row>
-    <row r="57" spans="1:13">
+      <c r="Q56" s="7" t="s">
+        <v>496</v>
+      </c>
+      <c r="S56" s="7" t="s">
+        <v>338</v>
+      </c>
+      <c r="T56" s="7">
+        <v>10</v>
+      </c>
+      <c r="U56" s="7" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="57" spans="1:21">
       <c r="A57" t="s">
         <v>12</v>
       </c>
@@ -6476,8 +7277,20 @@
       <c r="M57" s="2">
         <v>90.96</v>
       </c>
-    </row>
-    <row r="58" spans="1:13">
+      <c r="Q57" s="7" t="s">
+        <v>498</v>
+      </c>
+      <c r="S57" s="7" t="s">
+        <v>338</v>
+      </c>
+      <c r="T57" s="7">
+        <v>10</v>
+      </c>
+      <c r="U57" s="7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="58" spans="1:21">
       <c r="A58" t="s">
         <v>12</v>
       </c>
@@ -6514,8 +7327,20 @@
       <c r="M58" s="2">
         <v>19.2</v>
       </c>
-    </row>
-    <row r="59" spans="1:13">
+      <c r="Q58" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="S58" s="7" t="s">
+        <v>338</v>
+      </c>
+      <c r="T58" s="7">
+        <v>10</v>
+      </c>
+      <c r="U58" s="7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="59" spans="1:21">
       <c r="A59" t="s">
         <v>12</v>
       </c>
@@ -6552,8 +7377,20 @@
       <c r="M59" s="2">
         <v>38.4</v>
       </c>
-    </row>
-    <row r="60" spans="1:13">
+      <c r="Q59" s="7" t="s">
+        <v>528</v>
+      </c>
+      <c r="S59" s="7" t="s">
+        <v>338</v>
+      </c>
+      <c r="T59" s="7">
+        <v>10</v>
+      </c>
+      <c r="U59" s="7" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="60" spans="1:21">
       <c r="A60" t="s">
         <v>12</v>
       </c>
@@ -6593,8 +7430,20 @@
       <c r="M60" s="2">
         <v>80.88</v>
       </c>
-    </row>
-    <row r="61" spans="1:13">
+      <c r="Q60" s="7" t="s">
+        <v>565</v>
+      </c>
+      <c r="S60" s="7" t="s">
+        <v>338</v>
+      </c>
+      <c r="T60" s="7">
+        <v>10</v>
+      </c>
+      <c r="U60" s="7" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="61" spans="1:21">
       <c r="A61" t="s">
         <v>12</v>
       </c>
@@ -6631,8 +7480,20 @@
       <c r="M61" s="2">
         <v>8.64</v>
       </c>
-    </row>
-    <row r="62" spans="1:13">
+      <c r="Q61" s="7" t="s">
+        <v>579</v>
+      </c>
+      <c r="S61" s="7" t="s">
+        <v>402</v>
+      </c>
+      <c r="T61" s="7">
+        <v>20</v>
+      </c>
+      <c r="U61" s="7" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="62" spans="1:21">
       <c r="A62" t="s">
         <v>12</v>
       </c>
@@ -6669,8 +7530,20 @@
       <c r="M62" s="2">
         <v>55.2</v>
       </c>
-    </row>
-    <row r="63" spans="1:13">
+      <c r="Q62" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="S62" s="7" t="s">
+        <v>402</v>
+      </c>
+      <c r="T62" s="7">
+        <v>20</v>
+      </c>
+      <c r="U62" s="7" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="63" spans="1:21">
       <c r="A63" t="s">
         <v>12</v>
       </c>
@@ -6707,8 +7580,20 @@
       <c r="M63" s="2">
         <v>8.16</v>
       </c>
-    </row>
-    <row r="64" spans="1:13">
+      <c r="Q63" s="7" t="s">
+        <v>615</v>
+      </c>
+      <c r="S63" s="7" t="s">
+        <v>402</v>
+      </c>
+      <c r="T63" s="7">
+        <v>20</v>
+      </c>
+      <c r="U63" s="7" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="64" spans="1:21">
       <c r="A64" t="s">
         <v>12</v>
       </c>
@@ -6748,8 +7633,20 @@
       <c r="M64" s="2">
         <v>140.4</v>
       </c>
-    </row>
-    <row r="65" spans="1:13">
+      <c r="Q64" s="7" t="s">
+        <v>625</v>
+      </c>
+      <c r="S64" s="7" t="s">
+        <v>402</v>
+      </c>
+      <c r="T64" s="7">
+        <v>20</v>
+      </c>
+      <c r="U64" s="7" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="65" spans="1:21">
       <c r="A65" t="s">
         <v>12</v>
       </c>
@@ -6786,8 +7683,20 @@
       <c r="M65" s="2">
         <v>8.64</v>
       </c>
-    </row>
-    <row r="66" spans="1:13">
+      <c r="Q65" s="7" t="s">
+        <v>557</v>
+      </c>
+      <c r="S65" s="7" t="s">
+        <v>402</v>
+      </c>
+      <c r="T65" s="7">
+        <v>20</v>
+      </c>
+      <c r="U65" s="7" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="66" spans="1:21">
       <c r="A66" t="s">
         <v>12</v>
       </c>
@@ -6824,8 +7733,20 @@
       <c r="M66" s="2">
         <v>55.2</v>
       </c>
-    </row>
-    <row r="67" spans="1:13">
+      <c r="Q66" s="7" t="s">
+        <v>598</v>
+      </c>
+      <c r="S66" s="7" t="s">
+        <v>402</v>
+      </c>
+      <c r="T66" s="7">
+        <v>20</v>
+      </c>
+      <c r="U66" s="7" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="67" spans="1:21">
       <c r="A67" t="s">
         <v>12</v>
       </c>
@@ -6862,8 +7783,20 @@
       <c r="M67" s="2">
         <v>8.16</v>
       </c>
-    </row>
-    <row r="68" spans="1:13">
+      <c r="Q67" s="7" t="s">
+        <v>648</v>
+      </c>
+      <c r="S67" s="7" t="s">
+        <v>402</v>
+      </c>
+      <c r="T67" s="7">
+        <v>20</v>
+      </c>
+      <c r="U67" s="7" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="68" spans="1:21">
       <c r="A68" t="s">
         <v>12</v>
       </c>
@@ -6903,8 +7836,20 @@
       <c r="M68" s="2">
         <v>140.4</v>
       </c>
-    </row>
-    <row r="69" spans="1:13">
+      <c r="Q68" s="7" t="s">
+        <v>388</v>
+      </c>
+      <c r="S68" s="7" t="s">
+        <v>402</v>
+      </c>
+      <c r="T68" s="7">
+        <v>20</v>
+      </c>
+      <c r="U68" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="69" spans="1:21">
       <c r="A69" t="s">
         <v>12</v>
       </c>
@@ -6944,8 +7889,20 @@
       <c r="M69" s="2">
         <v>83.98</v>
       </c>
-    </row>
-    <row r="70" spans="1:13">
+      <c r="Q69" s="7" t="s">
+        <v>666</v>
+      </c>
+      <c r="S69" s="7" t="s">
+        <v>402</v>
+      </c>
+      <c r="T69" s="7">
+        <v>50</v>
+      </c>
+      <c r="U69" s="7" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="70" spans="1:21">
       <c r="A70" t="s">
         <v>12</v>
       </c>
@@ -6982,8 +7939,20 @@
       <c r="M70" s="2">
         <v>138.96</v>
       </c>
-    </row>
-    <row r="71" spans="1:13">
+      <c r="Q70" s="7" t="s">
+        <v>692</v>
+      </c>
+      <c r="S70" s="7" t="s">
+        <v>402</v>
+      </c>
+      <c r="T70" s="7">
+        <v>60</v>
+      </c>
+      <c r="U70" s="7" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="71" spans="1:21">
       <c r="A71" t="s">
         <v>12</v>
       </c>
@@ -7023,8 +7992,20 @@
       <c r="M71" s="2">
         <v>23.04</v>
       </c>
-    </row>
-    <row r="72" spans="1:13">
+      <c r="Q71" s="7" t="s">
+        <v>706</v>
+      </c>
+      <c r="S71" s="7" t="s">
+        <v>402</v>
+      </c>
+      <c r="T71" s="7">
+        <v>65</v>
+      </c>
+      <c r="U71" s="7" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="72" spans="1:21">
       <c r="A72" t="s">
         <v>12</v>
       </c>
@@ -7064,8 +8045,20 @@
       <c r="M72" s="2">
         <v>4.9800000000000004</v>
       </c>
-    </row>
-    <row r="73" spans="1:13">
+      <c r="Q72" s="7" t="s">
+        <v>729</v>
+      </c>
+      <c r="S72" s="7" t="s">
+        <v>402</v>
+      </c>
+      <c r="T72" s="7">
+        <v>80</v>
+      </c>
+      <c r="U72" s="7" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="73" spans="1:21">
       <c r="A73" t="s">
         <v>12</v>
       </c>
@@ -7105,8 +8098,20 @@
       <c r="M73" s="2">
         <v>162.24</v>
       </c>
-    </row>
-    <row r="74" spans="1:13">
+      <c r="Q73" s="7" t="s">
+        <v>739</v>
+      </c>
+      <c r="S73" s="7" t="s">
+        <v>402</v>
+      </c>
+      <c r="T73" s="7">
+        <v>80</v>
+      </c>
+      <c r="U73" s="7" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="74" spans="1:21">
       <c r="A74" t="s">
         <v>12</v>
       </c>
@@ -7146,8 +8151,20 @@
       <c r="M74" s="2">
         <v>162.24</v>
       </c>
-    </row>
-    <row r="75" spans="1:13">
+      <c r="Q74" s="7" t="s">
+        <v>755</v>
+      </c>
+      <c r="S74" s="7" t="s">
+        <v>402</v>
+      </c>
+      <c r="T74" s="7">
+        <v>101</v>
+      </c>
+      <c r="U74" s="7" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="75" spans="1:21">
       <c r="A75" t="s">
         <v>12</v>
       </c>
@@ -7187,8 +8204,20 @@
       <c r="M75" s="2">
         <v>202.2</v>
       </c>
-    </row>
-    <row r="76" spans="1:13">
+      <c r="Q75" s="7" t="s">
+        <v>215</v>
+      </c>
+      <c r="S75" s="7" t="s">
+        <v>402</v>
+      </c>
+      <c r="T75" s="7">
+        <v>110</v>
+      </c>
+      <c r="U75" s="7" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="76" spans="1:21">
       <c r="A76" t="s">
         <v>12</v>
       </c>
@@ -7228,8 +8257,20 @@
       <c r="M76" s="2">
         <v>202.2</v>
       </c>
-    </row>
-    <row r="77" spans="1:13">
+      <c r="Q76" s="7" t="s">
+        <v>780</v>
+      </c>
+      <c r="S76" s="7" t="s">
+        <v>402</v>
+      </c>
+      <c r="T76" s="7">
+        <v>117</v>
+      </c>
+      <c r="U76" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="77" spans="1:21">
       <c r="A77" t="s">
         <v>12</v>
       </c>
@@ -7269,8 +8310,20 @@
       <c r="M77" s="2">
         <v>80.88</v>
       </c>
-    </row>
-    <row r="78" spans="1:13">
+      <c r="Q77" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="S77" s="7" t="s">
+        <v>402</v>
+      </c>
+      <c r="T77" s="7">
+        <v>119</v>
+      </c>
+      <c r="U77" s="7" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="78" spans="1:21">
       <c r="A78" t="s">
         <v>12</v>
       </c>
@@ -7310,8 +8363,20 @@
       <c r="M78" s="2">
         <v>98</v>
       </c>
-    </row>
-    <row r="79" spans="1:13">
+      <c r="Q78" s="7" t="s">
+        <v>776</v>
+      </c>
+      <c r="S78" s="7" t="s">
+        <v>402</v>
+      </c>
+      <c r="T78" s="7">
+        <v>131</v>
+      </c>
+      <c r="U78" s="7" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="79" spans="1:21">
       <c r="A79" t="s">
         <v>12</v>
       </c>
@@ -7348,8 +8413,20 @@
       <c r="M79" s="2">
         <v>14.38</v>
       </c>
-    </row>
-    <row r="80" spans="1:13">
+      <c r="Q79" s="7" t="s">
+        <v>800</v>
+      </c>
+      <c r="S79" s="7" t="s">
+        <v>402</v>
+      </c>
+      <c r="T79" s="7">
+        <v>140</v>
+      </c>
+      <c r="U79" s="7" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="80" spans="1:21">
       <c r="A80" t="s">
         <v>12</v>
       </c>
@@ -7386,8 +8463,20 @@
       <c r="M80" s="2">
         <v>8.5</v>
       </c>
-    </row>
-    <row r="81" spans="1:13">
+      <c r="Q80" s="7" t="s">
+        <v>804</v>
+      </c>
+      <c r="S80" s="7" t="s">
+        <v>402</v>
+      </c>
+      <c r="T80" s="7">
+        <v>142</v>
+      </c>
+      <c r="U80" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="81" spans="1:21">
       <c r="A81" t="s">
         <v>12</v>
       </c>
@@ -7424,8 +8513,20 @@
       <c r="M81" s="2">
         <v>7.2</v>
       </c>
-    </row>
-    <row r="82" spans="1:13">
+      <c r="Q81" s="7" t="s">
+        <v>817</v>
+      </c>
+      <c r="S81" s="7" t="s">
+        <v>402</v>
+      </c>
+      <c r="T81" s="7">
+        <v>149</v>
+      </c>
+      <c r="U81" s="7" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="82" spans="1:21">
       <c r="A82" t="s">
         <v>12</v>
       </c>
@@ -7456,8 +8557,20 @@
       <c r="K82" s="2">
         <v>5.75</v>
       </c>
-    </row>
-    <row r="83" spans="1:13">
+      <c r="Q82" s="7" t="s">
+        <v>871</v>
+      </c>
+      <c r="S82" s="7" t="s">
+        <v>402</v>
+      </c>
+      <c r="T82" s="7">
+        <v>163</v>
+      </c>
+      <c r="U82" s="7" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="83" spans="1:21">
       <c r="A83" t="s">
         <v>12</v>
       </c>
@@ -7494,8 +8607,20 @@
       <c r="M83" s="2">
         <v>6.75</v>
       </c>
-    </row>
-    <row r="84" spans="1:13">
+      <c r="Q83" s="7" t="s">
+        <v>848</v>
+      </c>
+      <c r="S83" s="7" t="s">
+        <v>402</v>
+      </c>
+      <c r="T83" s="7">
+        <v>165</v>
+      </c>
+      <c r="U83" s="7" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="84" spans="1:21">
       <c r="A84" t="s">
         <v>12</v>
       </c>
@@ -7535,8 +8660,20 @@
       <c r="M84" s="2">
         <v>6</v>
       </c>
-    </row>
-    <row r="85" spans="1:13">
+      <c r="Q84" s="7" t="s">
+        <v>878</v>
+      </c>
+      <c r="S84" s="7" t="s">
+        <v>402</v>
+      </c>
+      <c r="T84" s="7">
+        <v>187</v>
+      </c>
+      <c r="U84" s="7" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="85" spans="1:21">
       <c r="A85" t="s">
         <v>12</v>
       </c>
@@ -7567,8 +8704,20 @@
       <c r="K85" s="2">
         <v>35.25</v>
       </c>
-    </row>
-    <row r="86" spans="1:13">
+      <c r="Q85" s="7" t="s">
+        <v>888</v>
+      </c>
+      <c r="S85" s="7" t="s">
+        <v>402</v>
+      </c>
+      <c r="T85" s="7" t="s">
+        <v>527</v>
+      </c>
+      <c r="U85" s="7" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="86" spans="1:21">
       <c r="A86" t="s">
         <v>12</v>
       </c>
@@ -7605,8 +8754,20 @@
       <c r="M86" s="2">
         <v>7.68</v>
       </c>
-    </row>
-    <row r="87" spans="1:13">
+      <c r="Q86" s="7" t="s">
+        <v>890</v>
+      </c>
+      <c r="S86" s="7" t="s">
+        <v>402</v>
+      </c>
+      <c r="T86" s="7" t="s">
+        <v>548</v>
+      </c>
+      <c r="U86" s="7" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="87" spans="1:21">
       <c r="A87" t="s">
         <v>12</v>
       </c>
@@ -7646,8 +8807,20 @@
       <c r="M87" s="2">
         <v>31.66</v>
       </c>
-    </row>
-    <row r="88" spans="1:13">
+      <c r="Q87" s="7" t="s">
+        <v>891</v>
+      </c>
+      <c r="S87" s="7" t="s">
+        <v>402</v>
+      </c>
+      <c r="T87" s="7" t="s">
+        <v>556</v>
+      </c>
+      <c r="U87" s="7" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="88" spans="1:21">
       <c r="A88" t="s">
         <v>12</v>
       </c>
@@ -7684,8 +8857,20 @@
       <c r="M88" s="2">
         <v>12.48</v>
       </c>
-    </row>
-    <row r="89" spans="1:13">
+      <c r="Q88" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="S88" s="7" t="s">
+        <v>402</v>
+      </c>
+      <c r="T88" s="7" t="s">
+        <v>577</v>
+      </c>
+      <c r="U88" s="7" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="89" spans="1:21">
       <c r="A89" t="s">
         <v>12</v>
       </c>
@@ -7722,8 +8907,20 @@
       <c r="M89" s="2">
         <v>7.2</v>
       </c>
-    </row>
-    <row r="90" spans="1:13">
+      <c r="Q89" s="7" t="s">
+        <v>898</v>
+      </c>
+      <c r="S89" s="7" t="s">
+        <v>402</v>
+      </c>
+      <c r="T89" s="7" t="s">
+        <v>585</v>
+      </c>
+      <c r="U89" s="7" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="90" spans="1:21">
       <c r="A90" t="s">
         <v>12</v>
       </c>
@@ -7760,8 +8957,20 @@
       <c r="M90" s="2">
         <v>7.48</v>
       </c>
-    </row>
-    <row r="91" spans="1:13">
+      <c r="Q90" s="7" t="s">
+        <v>909</v>
+      </c>
+      <c r="S90" s="7" t="s">
+        <v>402</v>
+      </c>
+      <c r="T90" s="7" t="s">
+        <v>597</v>
+      </c>
+      <c r="U90" s="7" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="91" spans="1:21">
       <c r="A91" t="s">
         <v>12</v>
       </c>
@@ -7801,8 +9010,20 @@
       <c r="M91" s="2">
         <v>17.760000000000002</v>
       </c>
-    </row>
-    <row r="92" spans="1:13">
+      <c r="Q91" s="7" t="s">
+        <v>919</v>
+      </c>
+      <c r="S91" s="7" t="s">
+        <v>635</v>
+      </c>
+      <c r="T91" s="7">
+        <v>52</v>
+      </c>
+      <c r="U91" s="7" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="92" spans="1:21">
       <c r="A92" t="s">
         <v>12</v>
       </c>
@@ -7839,8 +9060,20 @@
       <c r="M92" s="2">
         <v>7.68</v>
       </c>
-    </row>
-    <row r="93" spans="1:13">
+      <c r="Q92" s="7" t="s">
+        <v>922</v>
+      </c>
+      <c r="S92" s="7" t="s">
+        <v>635</v>
+      </c>
+      <c r="T92" s="7">
+        <v>54</v>
+      </c>
+      <c r="U92" s="7" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="93" spans="1:21">
       <c r="A93" t="s">
         <v>12</v>
       </c>
@@ -7877,8 +9110,20 @@
       <c r="M93" s="2">
         <v>7.2</v>
       </c>
-    </row>
-    <row r="94" spans="1:13">
+      <c r="Q93" s="7" t="s">
+        <v>925</v>
+      </c>
+      <c r="S93" s="7" t="s">
+        <v>635</v>
+      </c>
+      <c r="T93" s="7">
+        <v>56</v>
+      </c>
+      <c r="U93" s="7" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="94" spans="1:21">
       <c r="A94" t="s">
         <v>12</v>
       </c>
@@ -7915,8 +9160,20 @@
       <c r="M94" s="2">
         <v>12.48</v>
       </c>
-    </row>
-    <row r="95" spans="1:13">
+      <c r="Q94" s="7" t="s">
+        <v>942</v>
+      </c>
+      <c r="S94" s="7" t="s">
+        <v>635</v>
+      </c>
+      <c r="T94" s="7">
+        <v>100</v>
+      </c>
+      <c r="U94" s="7" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="95" spans="1:21">
       <c r="A95" t="s">
         <v>12</v>
       </c>
@@ -7956,8 +9213,20 @@
       <c r="M95" s="2">
         <v>11.02</v>
       </c>
-    </row>
-    <row r="96" spans="1:13">
+      <c r="Q95" s="7" t="s">
+        <v>947</v>
+      </c>
+      <c r="S95" s="7" t="s">
+        <v>635</v>
+      </c>
+      <c r="T95" s="7">
+        <v>104</v>
+      </c>
+      <c r="U95" s="7" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="96" spans="1:21">
       <c r="A96" t="s">
         <v>12</v>
       </c>
@@ -7997,8 +9266,20 @@
       <c r="M96" s="2">
         <v>9.84</v>
       </c>
-    </row>
-    <row r="97" spans="1:13">
+      <c r="Q96" s="7" t="s">
+        <v>981</v>
+      </c>
+      <c r="S96" s="7" t="s">
+        <v>635</v>
+      </c>
+      <c r="T96" s="7">
+        <v>117</v>
+      </c>
+      <c r="U96" s="7" t="s">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="97" spans="1:21">
       <c r="A97" t="s">
         <v>12</v>
       </c>
@@ -8035,8 +9316,20 @@
       <c r="M97" s="2">
         <v>8.14</v>
       </c>
-    </row>
-    <row r="98" spans="1:13">
+      <c r="Q97" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="S97" s="7" t="s">
+        <v>635</v>
+      </c>
+      <c r="T97" s="7">
+        <v>128</v>
+      </c>
+      <c r="U97" s="7" t="s">
+        <v>706</v>
+      </c>
+    </row>
+    <row r="98" spans="1:21">
       <c r="A98" t="s">
         <v>12</v>
       </c>
@@ -8073,8 +9366,20 @@
       <c r="M98" s="2">
         <v>7.2</v>
       </c>
-    </row>
-    <row r="99" spans="1:13">
+      <c r="Q98" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="S98" s="7" t="s">
+        <v>635</v>
+      </c>
+      <c r="T98" s="7">
+        <v>146</v>
+      </c>
+      <c r="U98" s="7" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="99" spans="1:21">
       <c r="A99" t="s">
         <v>12</v>
       </c>
@@ -8111,8 +9416,20 @@
       <c r="M99" s="2">
         <v>8.16</v>
       </c>
-    </row>
-    <row r="100" spans="1:13">
+      <c r="Q99" s="7" t="s">
+        <v>1002</v>
+      </c>
+      <c r="S99" s="7" t="s">
+        <v>635</v>
+      </c>
+      <c r="T99" s="7">
+        <v>161</v>
+      </c>
+      <c r="U99" s="7" t="s">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="100" spans="1:21">
       <c r="A100" t="s">
         <v>12</v>
       </c>
@@ -8149,8 +9466,20 @@
       <c r="M100" s="2">
         <v>8.5</v>
       </c>
-    </row>
-    <row r="101" spans="1:13">
+      <c r="Q100" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="S100" s="7" t="s">
+        <v>635</v>
+      </c>
+      <c r="T100" s="7">
+        <v>167</v>
+      </c>
+      <c r="U100" s="7" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="101" spans="1:21">
       <c r="A101" t="s">
         <v>12</v>
       </c>
@@ -8187,8 +9516,20 @@
       <c r="M101" s="2">
         <v>8.5</v>
       </c>
-    </row>
-    <row r="102" spans="1:13">
+      <c r="Q101" s="7" t="s">
+        <v>1010</v>
+      </c>
+      <c r="S101" s="7" t="s">
+        <v>635</v>
+      </c>
+      <c r="T101" s="7">
+        <v>176</v>
+      </c>
+      <c r="U101" s="7" t="s">
+        <v>755</v>
+      </c>
+    </row>
+    <row r="102" spans="1:21">
       <c r="A102" t="s">
         <v>12</v>
       </c>
@@ -8219,8 +9560,20 @@
       <c r="K102" s="2">
         <v>3.75</v>
       </c>
-    </row>
-    <row r="103" spans="1:13">
+      <c r="Q102" s="7" t="s">
+        <v>1008</v>
+      </c>
+      <c r="S102" s="7" t="s">
+        <v>635</v>
+      </c>
+      <c r="T102" s="7">
+        <v>177</v>
+      </c>
+      <c r="U102" s="7" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="103" spans="1:21">
       <c r="A103" t="s">
         <v>12</v>
       </c>
@@ -8260,8 +9613,20 @@
       <c r="M103" s="2">
         <v>6.5</v>
       </c>
-    </row>
-    <row r="104" spans="1:13">
+      <c r="Q103" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="S103" s="7" t="s">
+        <v>635</v>
+      </c>
+      <c r="T103" s="7">
+        <v>178</v>
+      </c>
+      <c r="U103" s="7" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="104" spans="1:21">
       <c r="A104" t="s">
         <v>12</v>
       </c>
@@ -8301,8 +9666,20 @@
       <c r="M104" s="2">
         <v>6</v>
       </c>
-    </row>
-    <row r="105" spans="1:13">
+      <c r="Q104" s="7" t="s">
+        <v>1015</v>
+      </c>
+      <c r="S104" s="7" t="s">
+        <v>635</v>
+      </c>
+      <c r="T104" s="7" t="s">
+        <v>527</v>
+      </c>
+      <c r="U104" s="7" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="105" spans="1:21">
       <c r="A105" t="s">
         <v>12</v>
       </c>
@@ -8342,8 +9719,20 @@
       <c r="M105" s="2">
         <v>13.98</v>
       </c>
-    </row>
-    <row r="106" spans="1:13">
+      <c r="Q105" s="7" t="s">
+        <v>634</v>
+      </c>
+      <c r="S105" s="7" t="s">
+        <v>635</v>
+      </c>
+      <c r="T105" s="7" t="s">
+        <v>712</v>
+      </c>
+      <c r="U105" s="7" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="106" spans="1:21">
       <c r="A106" t="s">
         <v>12</v>
       </c>
@@ -8380,8 +9769,20 @@
       <c r="M106" s="2">
         <v>20.14</v>
       </c>
-    </row>
-    <row r="107" spans="1:13">
+      <c r="Q106" s="7" t="s">
+        <v>1022</v>
+      </c>
+      <c r="S106" s="7" t="s">
+        <v>779</v>
+      </c>
+      <c r="T106" s="7">
+        <v>2</v>
+      </c>
+      <c r="U106" s="7" t="s">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="107" spans="1:21">
       <c r="A107" t="s">
         <v>12</v>
       </c>
@@ -8418,8 +9819,20 @@
       <c r="M107" s="2">
         <v>7.68</v>
       </c>
-    </row>
-    <row r="108" spans="1:13">
+      <c r="Q107" s="7" t="s">
+        <v>1027</v>
+      </c>
+      <c r="S107" s="7" t="s">
+        <v>779</v>
+      </c>
+      <c r="T107" s="7">
+        <v>44</v>
+      </c>
+      <c r="U107" s="7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="108" spans="1:21">
       <c r="A108" t="s">
         <v>12</v>
       </c>
@@ -8456,8 +9869,20 @@
       <c r="M108" s="2">
         <v>8.16</v>
       </c>
-    </row>
-    <row r="109" spans="1:13">
+      <c r="Q108" s="7" t="s">
+        <v>1031</v>
+      </c>
+      <c r="S108" s="7" t="s">
+        <v>786</v>
+      </c>
+      <c r="T108" s="7">
+        <v>10</v>
+      </c>
+      <c r="U108" s="7" t="s">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="109" spans="1:21">
       <c r="A109" t="s">
         <v>12</v>
       </c>
@@ -8488,8 +9913,20 @@
       <c r="K109" s="2">
         <v>24</v>
       </c>
-    </row>
-    <row r="110" spans="1:13">
+      <c r="Q109" s="7" t="s">
+        <v>1037</v>
+      </c>
+      <c r="S109" s="7" t="s">
+        <v>789</v>
+      </c>
+      <c r="T109" s="7">
+        <v>58</v>
+      </c>
+      <c r="U109" s="7" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="110" spans="1:21">
       <c r="A110" t="s">
         <v>12</v>
       </c>
@@ -8526,8 +9963,20 @@
       <c r="M110" s="2">
         <v>5.6</v>
       </c>
-    </row>
-    <row r="111" spans="1:13">
+      <c r="Q110" s="7" t="s">
+        <v>1040</v>
+      </c>
+      <c r="S110" s="7" t="s">
+        <v>789</v>
+      </c>
+      <c r="T110" s="7">
+        <v>62</v>
+      </c>
+      <c r="U110" s="7" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="111" spans="1:21">
       <c r="A111" t="s">
         <v>12</v>
       </c>
@@ -8558,8 +10007,20 @@
       <c r="K111" s="2">
         <v>30</v>
       </c>
-    </row>
-    <row r="112" spans="1:13">
+      <c r="Q111" s="7" t="s">
+        <v>1043</v>
+      </c>
+      <c r="S111" s="7" t="s">
+        <v>789</v>
+      </c>
+      <c r="T111" s="7">
+        <v>63</v>
+      </c>
+      <c r="U111" s="7" t="s">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="112" spans="1:21">
       <c r="A112" t="s">
         <v>12</v>
       </c>
@@ -8590,8 +10051,20 @@
       <c r="K112" s="2">
         <v>10.75</v>
       </c>
-    </row>
-    <row r="113" spans="1:13">
+      <c r="Q112" s="7" t="s">
+        <v>1064</v>
+      </c>
+      <c r="S112" s="7" t="s">
+        <v>789</v>
+      </c>
+      <c r="T112" s="7">
+        <v>65</v>
+      </c>
+      <c r="U112" s="7" t="s">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="113" spans="1:21">
       <c r="A113" t="s">
         <v>12</v>
       </c>
@@ -8622,8 +10095,20 @@
       <c r="K113" s="2">
         <v>2.25</v>
       </c>
-    </row>
-    <row r="114" spans="1:13">
+      <c r="Q113" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="S113" s="7" t="s">
+        <v>789</v>
+      </c>
+      <c r="T113" s="7">
+        <v>78</v>
+      </c>
+      <c r="U113" s="7" t="s">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="114" spans="1:21">
       <c r="A114" t="s">
         <v>12</v>
       </c>
@@ -8660,8 +10145,20 @@
       <c r="M114" s="2">
         <v>7.68</v>
       </c>
-    </row>
-    <row r="115" spans="1:13">
+      <c r="Q114" s="7" t="s">
+        <v>1083</v>
+      </c>
+      <c r="S114" s="7" t="s">
+        <v>789</v>
+      </c>
+      <c r="T114" s="7">
+        <v>97</v>
+      </c>
+      <c r="U114" s="7" t="s">
+        <v>817</v>
+      </c>
+    </row>
+    <row r="115" spans="1:21">
       <c r="A115" t="s">
         <v>12</v>
       </c>
@@ -8698,8 +10195,20 @@
       <c r="M115" s="2">
         <v>8.14</v>
       </c>
-    </row>
-    <row r="116" spans="1:13">
+      <c r="Q115" s="7" t="s">
+        <v>1089</v>
+      </c>
+      <c r="S115" s="7" t="s">
+        <v>789</v>
+      </c>
+      <c r="T115" s="7">
+        <v>98</v>
+      </c>
+      <c r="U115" s="7" t="s">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="116" spans="1:21">
       <c r="A116" t="s">
         <v>12</v>
       </c>
@@ -8730,8 +10239,20 @@
       <c r="K116" s="2">
         <v>6</v>
       </c>
-    </row>
-    <row r="117" spans="1:13">
+      <c r="Q116" s="7" t="s">
+        <v>1098</v>
+      </c>
+      <c r="S116" s="7" t="s">
+        <v>789</v>
+      </c>
+      <c r="T116" s="7">
+        <v>134</v>
+      </c>
+      <c r="U116" s="7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="117" spans="1:21">
       <c r="A117" t="s">
         <v>12</v>
       </c>
@@ -8768,8 +10289,17 @@
       <c r="M117" s="2">
         <v>5.26</v>
       </c>
-    </row>
-    <row r="118" spans="1:13">
+      <c r="S117" s="7" t="s">
+        <v>789</v>
+      </c>
+      <c r="T117" s="7">
+        <v>160</v>
+      </c>
+      <c r="U117" s="7" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="118" spans="1:21">
       <c r="A118" t="s">
         <v>12</v>
       </c>
@@ -8806,8 +10336,17 @@
       <c r="M118" s="2">
         <v>5.28</v>
       </c>
-    </row>
-    <row r="119" spans="1:13">
+      <c r="S118" s="7" t="s">
+        <v>789</v>
+      </c>
+      <c r="T118" s="7">
+        <v>163</v>
+      </c>
+      <c r="U118" s="7" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="119" spans="1:21">
       <c r="A119" t="s">
         <v>12</v>
       </c>
@@ -8838,8 +10377,17 @@
       <c r="K119" s="2">
         <v>3.75</v>
       </c>
-    </row>
-    <row r="120" spans="1:13">
+      <c r="S119" s="7" t="s">
+        <v>789</v>
+      </c>
+      <c r="T119" s="7">
+        <v>183</v>
+      </c>
+      <c r="U119" s="7" t="s">
+        <v>848</v>
+      </c>
+    </row>
+    <row r="120" spans="1:21">
       <c r="A120" t="s">
         <v>12</v>
       </c>
@@ -8876,8 +10424,17 @@
       <c r="M120" s="2">
         <v>7</v>
       </c>
-    </row>
-    <row r="121" spans="1:13">
+      <c r="S120" s="7" t="s">
+        <v>789</v>
+      </c>
+      <c r="T120" s="7">
+        <v>185</v>
+      </c>
+      <c r="U120" s="7" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="121" spans="1:21">
       <c r="A121" t="s">
         <v>12</v>
       </c>
@@ -8917,8 +10474,17 @@
       <c r="M121" s="2">
         <v>7.2</v>
       </c>
-    </row>
-    <row r="122" spans="1:13">
+      <c r="S121" s="7" t="s">
+        <v>789</v>
+      </c>
+      <c r="T121" s="7" t="s">
+        <v>830</v>
+      </c>
+      <c r="U121" s="7" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="122" spans="1:21">
       <c r="A122" t="s">
         <v>12</v>
       </c>
@@ -8955,8 +10521,17 @@
       <c r="M122" s="2">
         <v>3.98</v>
       </c>
-    </row>
-    <row r="123" spans="1:13">
+      <c r="S122" s="7" t="s">
+        <v>789</v>
+      </c>
+      <c r="T122" s="7" t="s">
+        <v>842</v>
+      </c>
+      <c r="U122" s="7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="123" spans="1:21">
       <c r="A123" t="s">
         <v>12</v>
       </c>
@@ -8993,8 +10568,17 @@
       <c r="M123" s="2">
         <v>6.75</v>
       </c>
-    </row>
-    <row r="124" spans="1:13">
+      <c r="S123" s="7" t="s">
+        <v>789</v>
+      </c>
+      <c r="T123" s="7" t="s">
+        <v>847</v>
+      </c>
+      <c r="U123" s="7" t="s">
+        <v>848</v>
+      </c>
+    </row>
+    <row r="124" spans="1:21">
       <c r="A124" t="s">
         <v>12</v>
       </c>
@@ -9034,8 +10618,17 @@
       <c r="M124" s="2">
         <v>6.5</v>
       </c>
-    </row>
-    <row r="125" spans="1:13">
+      <c r="S124" s="7" t="s">
+        <v>881</v>
+      </c>
+      <c r="T124" s="7">
+        <v>30</v>
+      </c>
+      <c r="U124" s="7" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="125" spans="1:21">
       <c r="A125" t="s">
         <v>12</v>
       </c>
@@ -9072,8 +10665,17 @@
       <c r="M125" s="2">
         <v>2.86</v>
       </c>
-    </row>
-    <row r="126" spans="1:13">
+      <c r="S125" s="7" t="s">
+        <v>881</v>
+      </c>
+      <c r="T125" s="7">
+        <v>30</v>
+      </c>
+      <c r="U125" s="7" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="126" spans="1:21">
       <c r="A126" t="s">
         <v>12</v>
       </c>
@@ -9113,8 +10715,17 @@
       <c r="M126" s="2">
         <v>6</v>
       </c>
-    </row>
-    <row r="127" spans="1:13">
+      <c r="S126" s="7" t="s">
+        <v>881</v>
+      </c>
+      <c r="T126" s="7">
+        <v>31</v>
+      </c>
+      <c r="U126" s="7" t="s">
+        <v>888</v>
+      </c>
+    </row>
+    <row r="127" spans="1:21">
       <c r="A127" t="s">
         <v>12</v>
       </c>
@@ -9145,8 +10756,17 @@
       <c r="K127" s="2">
         <v>5.25</v>
       </c>
-    </row>
-    <row r="128" spans="1:13">
+      <c r="S127" s="7" t="s">
+        <v>881</v>
+      </c>
+      <c r="T127" s="7">
+        <v>31</v>
+      </c>
+      <c r="U127" s="7" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="128" spans="1:21">
       <c r="A128" t="s">
         <v>12</v>
       </c>
@@ -9183,8 +10803,17 @@
       <c r="M128" s="2">
         <v>6.24</v>
       </c>
-    </row>
-    <row r="129" spans="1:13">
+      <c r="S128" s="7" t="s">
+        <v>881</v>
+      </c>
+      <c r="T128" s="7">
+        <v>32</v>
+      </c>
+      <c r="U128" s="7" t="s">
+        <v>891</v>
+      </c>
+    </row>
+    <row r="129" spans="1:21">
       <c r="A129" t="s">
         <v>12</v>
       </c>
@@ -9215,8 +10844,17 @@
       <c r="K129" s="2">
         <v>35.25</v>
       </c>
-    </row>
-    <row r="130" spans="1:13">
+      <c r="S129" s="7" t="s">
+        <v>881</v>
+      </c>
+      <c r="T129" s="7">
+        <v>32</v>
+      </c>
+      <c r="U129" s="7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="130" spans="1:21">
       <c r="A130" t="s">
         <v>12</v>
       </c>
@@ -9253,8 +10891,17 @@
       <c r="M130" s="2">
         <v>7.68</v>
       </c>
-    </row>
-    <row r="131" spans="1:13">
+      <c r="S130" s="7" t="s">
+        <v>881</v>
+      </c>
+      <c r="T130" s="7">
+        <v>60</v>
+      </c>
+      <c r="U130" s="7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="131" spans="1:21">
       <c r="A131" t="s">
         <v>12</v>
       </c>
@@ -9294,8 +10941,17 @@
       <c r="M131" s="2">
         <v>31.66</v>
       </c>
-    </row>
-    <row r="132" spans="1:13">
+      <c r="S131" s="7" t="s">
+        <v>881</v>
+      </c>
+      <c r="T131" s="7">
+        <v>111</v>
+      </c>
+      <c r="U131" s="7" t="s">
+        <v>898</v>
+      </c>
+    </row>
+    <row r="132" spans="1:21">
       <c r="A132" t="s">
         <v>12</v>
       </c>
@@ -9332,8 +10988,17 @@
       <c r="M132" s="2">
         <v>12.48</v>
       </c>
-    </row>
-    <row r="133" spans="1:13">
+      <c r="S132" s="7" t="s">
+        <v>881</v>
+      </c>
+      <c r="T132" s="7">
+        <v>131</v>
+      </c>
+      <c r="U132" s="7" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="133" spans="1:21">
       <c r="A133" t="s">
         <v>12</v>
       </c>
@@ -9370,8 +11035,17 @@
       <c r="M133" s="2">
         <v>7.2</v>
       </c>
-    </row>
-    <row r="134" spans="1:13">
+      <c r="S133" s="7" t="s">
+        <v>881</v>
+      </c>
+      <c r="T133" s="7">
+        <v>135</v>
+      </c>
+      <c r="U133" s="7" t="s">
+        <v>891</v>
+      </c>
+    </row>
+    <row r="134" spans="1:21">
       <c r="A134" t="s">
         <v>12</v>
       </c>
@@ -9408,8 +11082,17 @@
       <c r="M134" s="2">
         <v>7.48</v>
       </c>
-    </row>
-    <row r="135" spans="1:13">
+      <c r="S134" s="7" t="s">
+        <v>881</v>
+      </c>
+      <c r="T134" s="7">
+        <v>180</v>
+      </c>
+      <c r="U134" s="7" t="s">
+        <v>898</v>
+      </c>
+    </row>
+    <row r="135" spans="1:21">
       <c r="A135" t="s">
         <v>12</v>
       </c>
@@ -9449,8 +11132,17 @@
       <c r="M135" s="2">
         <v>17.760000000000002</v>
       </c>
-    </row>
-    <row r="136" spans="1:13">
+      <c r="S135" s="7" t="s">
+        <v>908</v>
+      </c>
+      <c r="T135" s="7">
+        <v>34</v>
+      </c>
+      <c r="U135" s="7" t="s">
+        <v>909</v>
+      </c>
+    </row>
+    <row r="136" spans="1:21">
       <c r="A136" t="s">
         <v>12</v>
       </c>
@@ -9490,8 +11182,17 @@
       <c r="M136" s="2">
         <v>98</v>
       </c>
-    </row>
-    <row r="137" spans="1:13">
+      <c r="S136" s="7" t="s">
+        <v>908</v>
+      </c>
+      <c r="T136" s="7">
+        <v>39</v>
+      </c>
+      <c r="U136" s="7" t="s">
+        <v>919</v>
+      </c>
+    </row>
+    <row r="137" spans="1:21">
       <c r="A137" t="s">
         <v>12</v>
       </c>
@@ -9531,8 +11232,17 @@
       <c r="M137" s="2">
         <v>168.72</v>
       </c>
-    </row>
-    <row r="138" spans="1:13">
+      <c r="S137" s="7" t="s">
+        <v>908</v>
+      </c>
+      <c r="T137" s="7">
+        <v>95</v>
+      </c>
+      <c r="U137" s="7" t="s">
+        <v>922</v>
+      </c>
+    </row>
+    <row r="138" spans="1:21">
       <c r="A138" t="s">
         <v>12</v>
       </c>
@@ -9566,8 +11276,17 @@
       <c r="K138" s="2">
         <v>169.25</v>
       </c>
-    </row>
-    <row r="139" spans="1:13">
+      <c r="S138" s="7" t="s">
+        <v>908</v>
+      </c>
+      <c r="T138" s="7">
+        <v>177</v>
+      </c>
+      <c r="U138" s="7" t="s">
+        <v>919</v>
+      </c>
+    </row>
+    <row r="139" spans="1:21">
       <c r="A139" t="s">
         <v>12</v>
       </c>
@@ -9601,8 +11320,17 @@
       <c r="K139" s="2">
         <v>116</v>
       </c>
-    </row>
-    <row r="140" spans="1:13">
+      <c r="S139" s="7" t="s">
+        <v>908</v>
+      </c>
+      <c r="T139" s="7">
+        <v>191</v>
+      </c>
+      <c r="U139" s="7" t="s">
+        <v>909</v>
+      </c>
+    </row>
+    <row r="140" spans="1:21">
       <c r="A140" t="s">
         <v>12</v>
       </c>
@@ -9636,8 +11364,17 @@
       <c r="K140" s="2">
         <v>169.25</v>
       </c>
-    </row>
-    <row r="141" spans="1:13">
+      <c r="S140" s="7" t="s">
+        <v>908</v>
+      </c>
+      <c r="T140" s="7" t="s">
+        <v>924</v>
+      </c>
+      <c r="U140" s="7" t="s">
+        <v>925</v>
+      </c>
+    </row>
+    <row r="141" spans="1:21">
       <c r="A141" t="s">
         <v>12</v>
       </c>
@@ -9671,8 +11408,17 @@
       <c r="K141" s="2">
         <v>116</v>
       </c>
-    </row>
-    <row r="142" spans="1:13">
+      <c r="S141" s="7" t="s">
+        <v>941</v>
+      </c>
+      <c r="T141" s="7">
+        <v>44</v>
+      </c>
+      <c r="U141" s="7" t="s">
+        <v>942</v>
+      </c>
+    </row>
+    <row r="142" spans="1:21">
       <c r="A142" t="s">
         <v>12</v>
       </c>
@@ -9709,8 +11455,17 @@
       <c r="M142" s="2">
         <v>6.84</v>
       </c>
-    </row>
-    <row r="143" spans="1:13">
+      <c r="S142" s="7" t="s">
+        <v>945</v>
+      </c>
+      <c r="T142" s="7" t="s">
+        <v>946</v>
+      </c>
+      <c r="U142" s="7" t="s">
+        <v>947</v>
+      </c>
+    </row>
+    <row r="143" spans="1:21">
       <c r="A143" t="s">
         <v>12</v>
       </c>
@@ -9747,8 +11502,17 @@
       <c r="M143" s="2">
         <v>6.12</v>
       </c>
-    </row>
-    <row r="144" spans="1:13">
+      <c r="S143" s="7" t="s">
+        <v>945</v>
+      </c>
+      <c r="T143" s="7" t="s">
+        <v>946</v>
+      </c>
+      <c r="U143" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="144" spans="1:21">
       <c r="A144" t="s">
         <v>12</v>
       </c>
@@ -9785,8 +11549,17 @@
       <c r="M144" s="2">
         <v>7.18</v>
       </c>
-    </row>
-    <row r="145" spans="1:13">
+      <c r="S144" s="7" t="s">
+        <v>945</v>
+      </c>
+      <c r="T144" s="7" t="s">
+        <v>961</v>
+      </c>
+      <c r="U144" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="145" spans="1:21">
       <c r="A145" t="s">
         <v>12</v>
       </c>
@@ -9823,8 +11596,17 @@
       <c r="M145" s="2">
         <v>5.26</v>
       </c>
-    </row>
-    <row r="146" spans="1:13">
+      <c r="S145" s="7" t="s">
+        <v>945</v>
+      </c>
+      <c r="T145" s="7" t="s">
+        <v>961</v>
+      </c>
+      <c r="U145" s="7" t="s">
+        <v>981</v>
+      </c>
+    </row>
+    <row r="146" spans="1:21">
       <c r="A146" t="s">
         <v>12</v>
       </c>
@@ -9855,8 +11637,17 @@
       <c r="K146" s="2">
         <v>8.25</v>
       </c>
-    </row>
-    <row r="147" spans="1:13">
+      <c r="S146" s="7" t="s">
+        <v>945</v>
+      </c>
+      <c r="T146" s="7" t="s">
+        <v>997</v>
+      </c>
+      <c r="U146" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="147" spans="1:21">
       <c r="A147" t="s">
         <v>12</v>
       </c>
@@ -9893,8 +11684,17 @@
       <c r="M147" s="2">
         <v>5.26</v>
       </c>
-    </row>
-    <row r="148" spans="1:13">
+      <c r="S147" s="7" t="s">
+        <v>945</v>
+      </c>
+      <c r="T147" s="7" t="s">
+        <v>997</v>
+      </c>
+      <c r="U147" s="7" t="s">
+        <v>981</v>
+      </c>
+    </row>
+    <row r="148" spans="1:21">
       <c r="A148" t="s">
         <v>12</v>
       </c>
@@ -9931,8 +11731,17 @@
       <c r="M148" s="2">
         <v>8.16</v>
       </c>
-    </row>
-    <row r="149" spans="1:13">
+      <c r="S148" s="7" t="s">
+        <v>998</v>
+      </c>
+      <c r="T148" s="7">
+        <v>30</v>
+      </c>
+      <c r="U148" s="7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="149" spans="1:21">
       <c r="A149" t="s">
         <v>12</v>
       </c>
@@ -9966,8 +11775,17 @@
       <c r="K149" s="2">
         <v>15</v>
       </c>
-    </row>
-    <row r="150" spans="1:13">
+      <c r="S149" s="7" t="s">
+        <v>998</v>
+      </c>
+      <c r="T149" s="7">
+        <v>30</v>
+      </c>
+      <c r="U149" s="7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="150" spans="1:21">
       <c r="A150" t="s">
         <v>12</v>
       </c>
@@ -10004,8 +11822,17 @@
       <c r="M150" s="2">
         <v>7.68</v>
       </c>
-    </row>
-    <row r="151" spans="1:13">
+      <c r="S150" s="7" t="s">
+        <v>998</v>
+      </c>
+      <c r="T150" s="7">
+        <v>30</v>
+      </c>
+      <c r="U150" s="7" t="s">
+        <v>1002</v>
+      </c>
+    </row>
+    <row r="151" spans="1:21">
       <c r="A151" t="s">
         <v>12</v>
       </c>
@@ -10042,8 +11869,17 @@
       <c r="M151" s="2">
         <v>12</v>
       </c>
-    </row>
-    <row r="152" spans="1:13">
+      <c r="S151" s="7" t="s">
+        <v>998</v>
+      </c>
+      <c r="T151" s="7">
+        <v>30</v>
+      </c>
+      <c r="U151" s="7" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="152" spans="1:21">
       <c r="A152" t="s">
         <v>12</v>
       </c>
@@ -10080,8 +11916,17 @@
       <c r="M152" s="2">
         <v>7.68</v>
       </c>
-    </row>
-    <row r="153" spans="1:13">
+      <c r="S152" s="7" t="s">
+        <v>998</v>
+      </c>
+      <c r="T152" s="7">
+        <v>37</v>
+      </c>
+      <c r="U152" s="7" t="s">
+        <v>1002</v>
+      </c>
+    </row>
+    <row r="153" spans="1:21">
       <c r="A153" t="s">
         <v>12</v>
       </c>
@@ -10118,8 +11963,17 @@
       <c r="M153" s="2">
         <v>5.26</v>
       </c>
-    </row>
-    <row r="154" spans="1:13">
+      <c r="S153" s="7" t="s">
+        <v>998</v>
+      </c>
+      <c r="T153" s="7">
+        <v>37</v>
+      </c>
+      <c r="U153" s="7" t="s">
+        <v>1010</v>
+      </c>
+    </row>
+    <row r="154" spans="1:21">
       <c r="A154" t="s">
         <v>12</v>
       </c>
@@ -10156,8 +12010,17 @@
       <c r="M154" s="2">
         <v>7.2</v>
       </c>
-    </row>
-    <row r="155" spans="1:13">
+      <c r="S154" s="7" t="s">
+        <v>998</v>
+      </c>
+      <c r="T154" s="7">
+        <v>37</v>
+      </c>
+      <c r="U154" s="7" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="155" spans="1:21">
       <c r="A155" t="s">
         <v>12</v>
       </c>
@@ -10194,8 +12057,17 @@
       <c r="M155" s="2">
         <v>9.98</v>
       </c>
-    </row>
-    <row r="156" spans="1:13">
+      <c r="S155" s="7" t="s">
+        <v>998</v>
+      </c>
+      <c r="T155" s="7">
+        <v>40</v>
+      </c>
+      <c r="U155" s="7" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="156" spans="1:21">
       <c r="A156" t="s">
         <v>12</v>
       </c>
@@ -10232,8 +12104,17 @@
       <c r="M156" s="2">
         <v>7.68</v>
       </c>
-    </row>
-    <row r="157" spans="1:13">
+      <c r="S156" s="7" t="s">
+        <v>998</v>
+      </c>
+      <c r="T156" s="7">
+        <v>65</v>
+      </c>
+      <c r="U156" s="7" t="s">
+        <v>1015</v>
+      </c>
+    </row>
+    <row r="157" spans="1:21">
       <c r="A157" t="s">
         <v>12</v>
       </c>
@@ -10270,8 +12151,17 @@
       <c r="M157" s="2">
         <v>7.2</v>
       </c>
-    </row>
-    <row r="158" spans="1:13">
+      <c r="S157" s="7" t="s">
+        <v>998</v>
+      </c>
+      <c r="T157" s="7">
+        <v>70</v>
+      </c>
+      <c r="U157" s="7" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="158" spans="1:21">
       <c r="A158" t="s">
         <v>12</v>
       </c>
@@ -10302,8 +12192,17 @@
       <c r="K158" s="2">
         <v>15</v>
       </c>
-    </row>
-    <row r="159" spans="1:13">
+      <c r="S158" s="7" t="s">
+        <v>998</v>
+      </c>
+      <c r="T158" s="7">
+        <v>81</v>
+      </c>
+      <c r="U158" s="7" t="s">
+        <v>1022</v>
+      </c>
+    </row>
+    <row r="159" spans="1:21">
       <c r="A159" t="s">
         <v>12</v>
       </c>
@@ -10340,8 +12239,17 @@
       <c r="M159" s="2">
         <v>11.52</v>
       </c>
-    </row>
-    <row r="160" spans="1:13">
+      <c r="S159" s="7" t="s">
+        <v>998</v>
+      </c>
+      <c r="T159" s="7">
+        <v>92</v>
+      </c>
+      <c r="U159" s="7" t="s">
+        <v>1002</v>
+      </c>
+    </row>
+    <row r="160" spans="1:21">
       <c r="A160" t="s">
         <v>12</v>
       </c>
@@ -10378,8 +12286,17 @@
       <c r="M160" s="2">
         <v>7.68</v>
       </c>
-    </row>
-    <row r="161" spans="1:13">
+      <c r="S160" s="7" t="s">
+        <v>998</v>
+      </c>
+      <c r="T160" s="7">
+        <v>109</v>
+      </c>
+      <c r="U160" s="7" t="s">
+        <v>1027</v>
+      </c>
+    </row>
+    <row r="161" spans="1:21">
       <c r="A161" t="s">
         <v>12</v>
       </c>
@@ -10416,8 +12333,17 @@
       <c r="M161" s="2">
         <v>8</v>
       </c>
-    </row>
-    <row r="162" spans="1:13">
+      <c r="S161" s="7" t="s">
+        <v>998</v>
+      </c>
+      <c r="T161" s="7">
+        <v>110</v>
+      </c>
+      <c r="U161" s="7" t="s">
+        <v>1031</v>
+      </c>
+    </row>
+    <row r="162" spans="1:21">
       <c r="A162" t="s">
         <v>12</v>
       </c>
@@ -10454,8 +12380,17 @@
       <c r="M162" s="2">
         <v>12.5</v>
       </c>
-    </row>
-    <row r="163" spans="1:13">
+      <c r="S162" s="7" t="s">
+        <v>998</v>
+      </c>
+      <c r="T162" s="7">
+        <v>120</v>
+      </c>
+      <c r="U162" s="7" t="s">
+        <v>1015</v>
+      </c>
+    </row>
+    <row r="163" spans="1:21">
       <c r="A163" t="s">
         <v>12</v>
       </c>
@@ -10486,8 +12421,17 @@
       <c r="K163" s="2">
         <v>15</v>
       </c>
-    </row>
-    <row r="164" spans="1:13">
+      <c r="S163" s="7" t="s">
+        <v>998</v>
+      </c>
+      <c r="T163" s="7">
+        <v>131</v>
+      </c>
+      <c r="U163" s="7" t="s">
+        <v>1037</v>
+      </c>
+    </row>
+    <row r="164" spans="1:21">
       <c r="A164" t="s">
         <v>12</v>
       </c>
@@ -10524,8 +12468,17 @@
       <c r="M164" s="2">
         <v>9.6</v>
       </c>
-    </row>
-    <row r="165" spans="1:13">
+      <c r="S164" s="7" t="s">
+        <v>998</v>
+      </c>
+      <c r="T164" s="7">
+        <v>140</v>
+      </c>
+      <c r="U164" s="7" t="s">
+        <v>1040</v>
+      </c>
+    </row>
+    <row r="165" spans="1:21">
       <c r="A165" t="s">
         <v>12</v>
       </c>
@@ -10556,8 +12509,17 @@
       <c r="K165" s="2">
         <v>4.5</v>
       </c>
-    </row>
-    <row r="166" spans="1:13">
+      <c r="S165" s="7" t="s">
+        <v>998</v>
+      </c>
+      <c r="T165" s="7">
+        <v>188</v>
+      </c>
+      <c r="U165" s="7" t="s">
+        <v>1043</v>
+      </c>
+    </row>
+    <row r="166" spans="1:21">
       <c r="A166" t="s">
         <v>12</v>
       </c>
@@ -10588,8 +12550,17 @@
       <c r="K166" s="2">
         <v>4.5</v>
       </c>
-    </row>
-    <row r="167" spans="1:13">
+      <c r="S166" s="7" t="s">
+        <v>1045</v>
+      </c>
+      <c r="T166" s="7">
+        <v>84</v>
+      </c>
+      <c r="U166" s="7" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="167" spans="1:21">
       <c r="A167" t="s">
         <v>12</v>
       </c>
@@ -10620,8 +12591,17 @@
       <c r="K167" s="2">
         <v>4.5</v>
       </c>
-    </row>
-    <row r="168" spans="1:13">
+      <c r="S167" s="7" t="s">
+        <v>1045</v>
+      </c>
+      <c r="T167" s="7">
+        <v>118</v>
+      </c>
+      <c r="U167" s="7" t="s">
+        <v>1064</v>
+      </c>
+    </row>
+    <row r="168" spans="1:21">
       <c r="A168" t="s">
         <v>12</v>
       </c>
@@ -10652,8 +12632,17 @@
       <c r="K168" s="2">
         <v>4.5</v>
       </c>
-    </row>
-    <row r="169" spans="1:13">
+      <c r="S168" s="7" t="s">
+        <v>1045</v>
+      </c>
+      <c r="T168" s="7">
+        <v>165</v>
+      </c>
+      <c r="U168" s="7" t="s">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="169" spans="1:21">
       <c r="A169" t="s">
         <v>12</v>
       </c>
@@ -10684,8 +12673,17 @@
       <c r="K169" s="2">
         <v>4.5</v>
       </c>
-    </row>
-    <row r="170" spans="1:13">
+      <c r="S169" s="7" t="s">
+        <v>1045</v>
+      </c>
+      <c r="T169" s="7" t="s">
+        <v>1072</v>
+      </c>
+      <c r="U169" s="7" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="170" spans="1:21">
       <c r="A170" t="s">
         <v>12</v>
       </c>
@@ -10722,8 +12720,17 @@
       <c r="M170" s="2">
         <v>6.38</v>
       </c>
-    </row>
-    <row r="171" spans="1:13">
+      <c r="S170" s="7" t="s">
+        <v>1084</v>
+      </c>
+      <c r="T170" s="7">
+        <v>2</v>
+      </c>
+      <c r="U170" s="7" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="171" spans="1:21">
       <c r="A171" t="s">
         <v>12</v>
       </c>
@@ -10760,8 +12767,17 @@
       <c r="M171" s="2">
         <v>7.68</v>
       </c>
-    </row>
-    <row r="172" spans="1:13">
+      <c r="S171" s="7" t="s">
+        <v>1084</v>
+      </c>
+      <c r="T171" s="7">
+        <v>22</v>
+      </c>
+      <c r="U171" s="7" t="s">
+        <v>1083</v>
+      </c>
+    </row>
+    <row r="172" spans="1:21">
       <c r="A172" t="s">
         <v>12</v>
       </c>
@@ -10798,8 +12814,17 @@
       <c r="M172" s="2">
         <v>5.98</v>
       </c>
-    </row>
-    <row r="173" spans="1:13">
+      <c r="S172" s="7" t="s">
+        <v>1084</v>
+      </c>
+      <c r="T172" s="7">
+        <v>33</v>
+      </c>
+      <c r="U172" s="7" t="s">
+        <v>1089</v>
+      </c>
+    </row>
+    <row r="173" spans="1:21">
       <c r="A173" t="s">
         <v>12</v>
       </c>
@@ -10836,8 +12861,17 @@
       <c r="M173" s="2">
         <v>7.66</v>
       </c>
-    </row>
-    <row r="174" spans="1:13">
+      <c r="S173" s="7" t="s">
+        <v>1084</v>
+      </c>
+      <c r="T173" s="7">
+        <v>33</v>
+      </c>
+      <c r="U173" s="7" t="s">
+        <v>1083</v>
+      </c>
+    </row>
+    <row r="174" spans="1:21">
       <c r="A174" t="s">
         <v>12</v>
       </c>
@@ -10874,8 +12908,17 @@
       <c r="M174" s="2">
         <v>7.2</v>
       </c>
-    </row>
-    <row r="175" spans="1:13">
+      <c r="S174" s="7" t="s">
+        <v>1084</v>
+      </c>
+      <c r="T174" s="7">
+        <v>44</v>
+      </c>
+      <c r="U174" s="7" t="s">
+        <v>1089</v>
+      </c>
+    </row>
+    <row r="175" spans="1:21">
       <c r="A175" t="s">
         <v>12</v>
       </c>
@@ -10906,8 +12949,17 @@
       <c r="K175" s="2">
         <v>4.5</v>
       </c>
-    </row>
-    <row r="176" spans="1:13">
+      <c r="S175" s="7" t="s">
+        <v>1084</v>
+      </c>
+      <c r="T175" s="7">
+        <v>158</v>
+      </c>
+      <c r="U175" s="7" t="s">
+        <v>1098</v>
+      </c>
+    </row>
+    <row r="176" spans="1:21">
       <c r="A176" t="s">
         <v>12</v>
       </c>
@@ -10944,8 +12996,17 @@
       <c r="M176" s="2">
         <v>6.7</v>
       </c>
-    </row>
-    <row r="177" spans="1:13">
+      <c r="S176" s="7" t="s">
+        <v>1084</v>
+      </c>
+      <c r="T176" s="7" t="s">
+        <v>1095</v>
+      </c>
+      <c r="U176" s="7" t="s">
+        <v>942</v>
+      </c>
+    </row>
+    <row r="177" spans="1:20">
       <c r="A177" t="s">
         <v>12</v>
       </c>
@@ -10976,8 +13037,10 @@
       <c r="K177" s="2">
         <v>23.25</v>
       </c>
-    </row>
-    <row r="178" spans="1:13">
+      <c r="S177" s="7"/>
+      <c r="T177" s="7"/>
+    </row>
+    <row r="178" spans="1:20">
       <c r="A178" t="s">
         <v>12</v>
       </c>
@@ -11015,7 +13078,7 @@
         <v>7.68</v>
       </c>
     </row>
-    <row r="179" spans="1:13">
+    <row r="179" spans="1:20">
       <c r="A179" t="s">
         <v>12</v>
       </c>
@@ -11056,7 +13119,7 @@
         <v>17.260000000000002</v>
       </c>
     </row>
-    <row r="180" spans="1:13">
+    <row r="180" spans="1:20">
       <c r="A180" t="s">
         <v>12</v>
       </c>
@@ -11088,7 +13151,7 @@
         <v>12.75</v>
       </c>
     </row>
-    <row r="181" spans="1:13">
+    <row r="181" spans="1:20">
       <c r="A181" t="s">
         <v>12</v>
       </c>
@@ -11129,7 +13192,7 @@
         <v>39.119999999999997</v>
       </c>
     </row>
-    <row r="182" spans="1:13">
+    <row r="182" spans="1:20">
       <c r="A182" t="s">
         <v>12</v>
       </c>
@@ -11170,7 +13233,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="183" spans="1:13">
+    <row r="183" spans="1:20">
       <c r="A183" t="s">
         <v>12</v>
       </c>
@@ -11208,7 +13271,7 @@
         <v>8.16</v>
       </c>
     </row>
-    <row r="184" spans="1:13">
+    <row r="184" spans="1:20">
       <c r="A184" t="s">
         <v>12</v>
       </c>
@@ -11246,7 +13309,7 @@
         <v>7.68</v>
       </c>
     </row>
-    <row r="185" spans="1:13">
+    <row r="185" spans="1:20">
       <c r="A185" t="s">
         <v>12</v>
       </c>
@@ -11287,7 +13350,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="186" spans="1:13">
+    <row r="186" spans="1:20">
       <c r="A186" t="s">
         <v>12</v>
       </c>
@@ -11325,7 +13388,7 @@
         <v>9.1</v>
       </c>
     </row>
-    <row r="187" spans="1:13">
+    <row r="187" spans="1:20">
       <c r="A187" t="s">
         <v>12</v>
       </c>
@@ -11363,7 +13426,7 @@
         <v>4.32</v>
       </c>
     </row>
-    <row r="188" spans="1:13">
+    <row r="188" spans="1:20">
       <c r="A188" t="s">
         <v>12</v>
       </c>
@@ -11401,7 +13464,7 @@
         <v>9.1</v>
       </c>
     </row>
-    <row r="189" spans="1:13">
+    <row r="189" spans="1:20">
       <c r="A189" t="s">
         <v>12</v>
       </c>
@@ -11439,7 +13502,7 @@
         <v>4.32</v>
       </c>
     </row>
-    <row r="190" spans="1:13">
+    <row r="190" spans="1:20">
       <c r="A190" t="s">
         <v>12</v>
       </c>
@@ -11480,7 +13543,7 @@
         <v>75.84</v>
       </c>
     </row>
-    <row r="191" spans="1:13">
+    <row r="191" spans="1:20">
       <c r="A191" t="s">
         <v>12</v>
       </c>
@@ -11518,7 +13581,7 @@
         <v>12.48</v>
       </c>
     </row>
-    <row r="192" spans="1:13">
+    <row r="192" spans="1:20">
       <c r="A192" t="s">
         <v>12</v>
       </c>
@@ -29242,11 +31305,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M661">
-    <sortState ref="A2:R3039">
-      <sortCondition ref="A1:A3039"/>
-    </sortState>
-  </autoFilter>
+  <autoFilter ref="A1:M660"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>

</xml_diff>